<commit_message>
last button studenti page added
</commit_message>
<xml_diff>
--- a/ExamManagerApplication/ExamManager/ExamManager.Web/Files/testStudentImport.xlsx
+++ b/ExamManagerApplication/ExamManager/ExamManager.Web/Files/testStudentImport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simona\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JMarkovikj\source\repos\ExamManager1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD9F0D4A-97EB-4D31-B40D-31ABD357E0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA5EC27-60F9-4446-9755-B268808B35DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CEC2EE0F-466F-4035-B7BB-A304179C2FB2}"/>
   </bookViews>
@@ -37,28 +37,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>TestIme</t>
-  </si>
-  <si>
-    <t>TestIme1</t>
-  </si>
-  <si>
-    <t>TestIme2</t>
-  </si>
-  <si>
-    <t>TestIme3</t>
-  </si>
-  <si>
-    <t>TestIme4</t>
-  </si>
-  <si>
-    <t>TestIme5</t>
-  </si>
-  <si>
-    <t>TestIme7</t>
-  </si>
-  <si>
-    <t>TestIme6</t>
+    <t>ATestIme</t>
+  </si>
+  <si>
+    <t>ATestIme1</t>
+  </si>
+  <si>
+    <t>ATestIme2</t>
+  </si>
+  <si>
+    <t>ATestIme3</t>
+  </si>
+  <si>
+    <t>ATestIme4</t>
+  </si>
+  <si>
+    <t>ATestIme5</t>
+  </si>
+  <si>
+    <t>ATestIme6</t>
+  </si>
+  <si>
+    <t>ATestIme7</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,7 +468,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>542361</v>
@@ -476,7 +476,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>542362</v>

</xml_diff>